<commit_message>
Update import student, kan nu een of meerdere groepen toevoegen
</commit_message>
<xml_diff>
--- a/Barometer VS Project/Barometer_ASP_NET/Barometer_ASP_NET/Content/ExcelTemplates/StudentTemplate.xlsx
+++ b/Barometer VS Project/Barometer_ASP_NET/Barometer_ASP_NET/Content/ExcelTemplates/StudentTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Dropbox\School\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Leaping-Cliff\Barometer VS Project\Barometer_ASP_NET\Barometer_ASP_NET\Content\ExcelTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Studentnummer</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Emailadres</t>
+  </si>
+  <si>
+    <t>Groepnaam</t>
   </si>
 </sst>
 </file>
@@ -353,10 +356,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E1048576"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -365,9 +368,10 @@
     <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.28515625" customWidth="1"/>
     <col min="4" max="4" width="64.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,6 +383,9 @@
       </c>
       <c r="D1" t="s">
         <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>